<commit_message>
fix font + fix about + added more data
</commit_message>
<xml_diff>
--- a/data/teamers_data.xlsx
+++ b/data/teamers_data.xlsx
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -486,396 +486,396 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.8235294117647058</v>
       </c>
       <c r="E3" t="n">
-        <v>1.111111111111111</v>
+        <v>1.176470588235294</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sundiata-Keita</t>
+          <t>Ramses</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.8</v>
       </c>
       <c r="E4" t="n">
-        <v>1.142857142857143</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ramses</t>
+          <t>Catherine-Magnificence</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="E5" t="n">
-        <v>1.2</v>
+        <v>1.266666666666667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Sundiata-Keita</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D6" t="n">
-        <v>0.75</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="E6" t="n">
-        <v>1.25</v>
+        <v>1.294117647058824</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Eleanor-En</t>
+          <t>Maori</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="E7" t="n">
-        <v>1.272727272727273</v>
+        <v>1.304347826086957</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Catherine-Magnificence</t>
+          <t>Eleanor-En</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="E8" t="n">
-        <v>1.285714285714286</v>
+        <v>1.307692307692308</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gran-Colombia</t>
+          <t>Gandhi</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="E9" t="n">
-        <v>1.294117647058824</v>
+        <v>1.307692307692308</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Harald-Varangian</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6756756756756757</v>
       </c>
       <c r="E10" t="n">
-        <v>1.333333333333333</v>
+        <v>1.324324324324324</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Gandhi</t>
+          <t>Mvemba-a-Nzinga</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="E11" t="n">
-        <v>1.333333333333333</v>
+        <v>1.357142857142857</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mvemba-a-Nzinga</t>
+          <t>Eleanor-Fr</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="E12" t="n">
-        <v>1.333333333333333</v>
+        <v>1.357142857142857</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Nubia</t>
+          <t>Rome</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C13" t="n">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6212121212121212</v>
       </c>
       <c r="E13" t="n">
-        <v>1.333333333333333</v>
+        <v>1.363636363636364</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cree</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E14" t="n">
-        <v>1.347826086956522</v>
+        <v>1.388888888888889</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Scotland</t>
+          <t>Tokugawa</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C15" t="n">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="D15" t="n">
-        <v>0.625</v>
+        <v>0.6078431372549019</v>
       </c>
       <c r="E15" t="n">
-        <v>1.375</v>
+        <v>1.392156862745098</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Maori</t>
+          <t>Cree</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C16" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D16" t="n">
-        <v>0.625</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="E16" t="n">
-        <v>1.375</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kublai-Mongolia</t>
+          <t>Victoria</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C17" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D17" t="n">
-        <v>0.62</v>
+        <v>0.575</v>
       </c>
       <c r="E17" t="n">
-        <v>1.38</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Mbande</t>
+          <t>Kublai-Mongolia</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C18" t="n">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5384615384615384</v>
+        <v>0.5945945945945946</v>
       </c>
       <c r="E18" t="n">
-        <v>1.384615384615385</v>
+        <v>1.405405405405405</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Suleiman-Muhtesem</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6153846153846154</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="E19" t="n">
-        <v>1.384615384615385</v>
+        <v>1.411764705882353</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Tokugawa</t>
+          <t>Persia</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C20" t="n">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6153846153846154</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E20" t="n">
-        <v>1.384615384615385</v>
+        <v>1.416666666666667</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Eleanor-Fr</t>
+          <t>Mbande</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C21" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6153846153846154</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="E21" t="n">
-        <v>1.384615384615385</v>
+        <v>1.421052631578947</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Korea</t>
+          <t>Julius-Caesar</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" t="n">
         <v>26</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6153846153846154</v>
+        <v>0.5769230769230769</v>
       </c>
       <c r="E22" t="n">
-        <v>1.384615384615385</v>
+        <v>1.423076923076923</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Byzantium</t>
+          <t>Scotland</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D23" t="n">
-        <v>0.6</v>
+        <v>0.5769230769230769</v>
       </c>
       <c r="E23" t="n">
-        <v>1.4</v>
+        <v>1.423076923076923</v>
       </c>
     </row>
     <row r="24">
@@ -885,314 +885,314 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C24" t="n">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6</v>
+        <v>0.5681818181818182</v>
       </c>
       <c r="E24" t="n">
-        <v>1.4</v>
+        <v>1.431818181818182</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Rome</t>
+          <t>Ethiopia</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C25" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D25" t="n">
-        <v>0.575</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="E25" t="n">
-        <v>1.425</v>
+        <v>1.433333333333333</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Suleiman-Kanuni</t>
+          <t>Wu-Zetian</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C26" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D26" t="n">
-        <v>0.575</v>
+        <v>0.5588235294117647</v>
       </c>
       <c r="E26" t="n">
-        <v>1.425</v>
+        <v>1.441176470588235</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Macedon</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C27" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E27" t="n">
-        <v>1.428571428571429</v>
+        <v>1.444444444444444</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Suleiman-Muhtesem</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C28" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E28" t="n">
-        <v>1.428571428571429</v>
+        <v>1.444444444444444</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Genghis-Khan</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C29" t="n">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.5405405405405406</v>
       </c>
       <c r="E29" t="n">
-        <v>1.428571428571429</v>
+        <v>1.459459459459459</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Babylon</t>
+          <t>Gorgo</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5652173913043478</v>
+        <v>0.5370370370370371</v>
       </c>
       <c r="E30" t="n">
-        <v>1.434782608695652</v>
+        <v>1.462962962962963</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Qin-Unifier</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C31" t="n">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5319148936170213</v>
       </c>
       <c r="E31" t="n">
-        <v>1.444444444444444</v>
+        <v>1.468085106382979</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Wu-Zetian</t>
+          <t>Gran-Colombia</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C32" t="n">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D32" t="n">
-        <v>0.55</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="E32" t="n">
-        <v>1.45</v>
+        <v>1.473684210526316</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Gorgo</t>
+          <t>Macedon</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5428571428571428</v>
+        <v>0.5217391304347826</v>
       </c>
       <c r="E33" t="n">
-        <v>1.457142857142857</v>
+        <v>1.478260869565217</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Scythia</t>
+          <t>Nubia</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5384615384615384</v>
+        <v>0.52</v>
       </c>
       <c r="E34" t="n">
-        <v>1.461538461538461</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Suleiman-Kanuni</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C35" t="n">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D35" t="n">
-        <v>0.53125</v>
+        <v>0.5161290322580645</v>
       </c>
       <c r="E35" t="n">
-        <v>1.46875</v>
+        <v>1.483870967741935</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Ethiopia</t>
+          <t>Korea</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C36" t="n">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D36" t="n">
-        <v>0.5294117647058824</v>
+        <v>0.5135135135135135</v>
       </c>
       <c r="E36" t="n">
-        <v>1.470588235294118</v>
+        <v>1.486486486486486</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Pericles</t>
+          <t>Harald-Varangian</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C37" t="n">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D37" t="n">
-        <v>0.5294117647058824</v>
+        <v>0.5135135135135135</v>
       </c>
       <c r="E37" t="n">
-        <v>1.470588235294118</v>
+        <v>1.486486486486486</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Chandragupta</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C38" t="n">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D38" t="n">
-        <v>0.5185185185185185</v>
+        <v>0.5111111111111111</v>
       </c>
       <c r="E38" t="n">
-        <v>1.481481481481481</v>
+        <v>1.488888888888889</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Victoria</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C39" t="n">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5128205128205128</v>
+        <v>0.5076923076923077</v>
       </c>
       <c r="E39" t="n">
-        <v>1.487179487179487</v>
+        <v>1.492307692307692</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Persia</t>
+          <t>Pericles</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C40" t="n">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D40" t="n">
         <v>0.5</v>
@@ -1204,14 +1204,14 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Qin-Unifier</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C41" t="n">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D41" t="n">
         <v>0.5</v>
@@ -1223,14 +1223,14 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Nader-Shah</t>
+          <t>Catherine-BQ</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C42" t="n">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="D42" t="n">
         <v>0.5</v>
@@ -1242,14 +1242,14 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Kublai-China</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C43" t="n">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D43" t="n">
         <v>0.5</v>
@@ -1261,14 +1261,14 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mali</t>
+          <t>Teddy-RR</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D44" t="n">
         <v>0.5</v>
@@ -1280,508 +1280,508 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Catherine-BQ</t>
+          <t>ElizabethI</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C45" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D45" t="n">
-        <v>0.4871794871794872</v>
+        <v>0.5</v>
       </c>
       <c r="E45" t="n">
-        <v>1.512820512820513</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Aztec</t>
+          <t>Gaul</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C46" t="n">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D46" t="n">
-        <v>0.4705882352941176</v>
+        <v>0.5</v>
       </c>
       <c r="E46" t="n">
-        <v>1.529411764705882</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Kublai-China</t>
+          <t>Aztec</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C47" t="n">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D47" t="n">
-        <v>0.4705882352941176</v>
+        <v>0.4905660377358491</v>
       </c>
       <c r="E47" t="n">
-        <v>1.529411764705882</v>
+        <v>1.509433962264151</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C48" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D48" t="n">
-        <v>0.46875</v>
+        <v>0.4883720930232558</v>
       </c>
       <c r="E48" t="n">
-        <v>1.53125</v>
+        <v>1.511627906976744</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Chandragupta</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C49" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D49" t="n">
-        <v>0.46875</v>
+        <v>0.4883720930232558</v>
       </c>
       <c r="E49" t="n">
-        <v>1.53125</v>
+        <v>1.511627906976744</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Victoria age of steam</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C50" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D50" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.4878048780487805</v>
       </c>
       <c r="E50" t="n">
-        <v>1.533333333333333</v>
+        <v>1.51219512195122</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Scythia</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C51" t="n">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D51" t="n">
-        <v>0.4642857142857143</v>
+        <v>0.4878048780487805</v>
       </c>
       <c r="E51" t="n">
-        <v>1.535714285714286</v>
+        <v>1.51219512195122</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Nader-Shah</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C52" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D52" t="n">
-        <v>0.4615384615384616</v>
+        <v>0.4838709677419355</v>
       </c>
       <c r="E52" t="n">
-        <v>1.538461538461539</v>
+        <v>1.516129032258065</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Zulu</t>
+          <t>Sumeria</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C53" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D53" t="n">
-        <v>0.4615384615384616</v>
+        <v>0.4827586206896552</v>
       </c>
       <c r="E53" t="n">
-        <v>1.538461538461539</v>
+        <v>1.517241379310345</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C54" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D54" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4814814814814815</v>
       </c>
       <c r="E54" t="n">
-        <v>1.541666666666667</v>
+        <v>1.518518518518519</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Gaul</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C55" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D55" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E55" t="n">
-        <v>1.541666666666667</v>
+        <v>1.520833333333333</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Julius-Caesar</t>
+          <t>Babylon</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C56" t="n">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D56" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="E56" t="n">
-        <v>1.545454545454545</v>
+        <v>1.523809523809524</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C57" t="n">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D57" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.4727272727272727</v>
       </c>
       <c r="E57" t="n">
-        <v>1.545454545454545</v>
+        <v>1.527272727272727</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Hojo-Tokimune</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C58" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D58" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="E58" t="n">
-        <v>1.545454545454545</v>
+        <v>1.538461538461539</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Victoria age of steam</t>
+          <t>Hojo-Tokimune</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C59" t="n">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D59" t="n">
-        <v>0.4482758620689655</v>
+        <v>0.4516129032258064</v>
       </c>
       <c r="E59" t="n">
-        <v>1.551724137931034</v>
+        <v>1.548387096774194</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ElizabethI</t>
+          <t>Phoenicia</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C60" t="n">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D60" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.4347826086956522</v>
       </c>
       <c r="E60" t="n">
-        <v>1.555555555555556</v>
+        <v>1.565217391304348</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Byzantium</t>
         </is>
       </c>
       <c r="B61" t="n">
+        <v>3</v>
+      </c>
+      <c r="C61" t="n">
         <v>7</v>
       </c>
-      <c r="C61" t="n">
-        <v>16</v>
-      </c>
       <c r="D61" t="n">
-        <v>0.4375</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="E61" t="n">
-        <v>1.5625</v>
+        <v>1.571428571428571</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Teddy-RR</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C62" t="n">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="D62" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.4107142857142857</v>
       </c>
       <c r="E62" t="n">
-        <v>1.571428571428571</v>
+        <v>1.589285714285714</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Theodora</t>
+          <t>Mapuche</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C63" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D63" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.4090909090909091</v>
       </c>
       <c r="E63" t="n">
-        <v>1.571428571428571</v>
+        <v>1.590909090909091</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Phoenicia</t>
+          <t>Inca</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C64" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.4</v>
       </c>
       <c r="E64" t="n">
-        <v>1.571428571428571</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Saladin-Sultan</t>
         </is>
       </c>
       <c r="B65" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" t="n">
         <v>10</v>
       </c>
-      <c r="C65" t="n">
-        <v>24</v>
-      </c>
       <c r="D65" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="E65" t="n">
-        <v>1.583333333333333</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Inca</t>
+          <t>Qin-Mandate-of-Heaven</t>
         </is>
       </c>
       <c r="B66" t="n">
+        <v>2</v>
+      </c>
+      <c r="C66" t="n">
         <v>5</v>
       </c>
-      <c r="C66" t="n">
-        <v>13</v>
-      </c>
       <c r="D66" t="n">
-        <v>0.3846153846153846</v>
+        <v>0.4</v>
       </c>
       <c r="E66" t="n">
-        <v>1.615384615384615</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sumeria</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C67" t="n">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D67" t="n">
-        <v>0.375</v>
+        <v>0.4</v>
       </c>
       <c r="E67" t="n">
-        <v>1.625</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Genghis-Khan</t>
+          <t>Teddy-BM</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C68" t="n">
         <v>20</v>
       </c>
       <c r="D68" t="n">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="E68" t="n">
-        <v>1.65</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Saladin-Sultan</t>
+          <t>Zulu</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C69" t="n">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="D69" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3809523809523809</v>
       </c>
       <c r="E69" t="n">
-        <v>1.666666666666667</v>
+        <v>1.619047619047619</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Teddy-BM</t>
+          <t>Yongle</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C70" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D70" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3571428571428572</v>
       </c>
       <c r="E70" t="n">
-        <v>1.666666666666667</v>
+        <v>1.642857142857143</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Qin-Mandate-of-Heaven</t>
+          <t>Ludwig</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C71" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D71" t="n">
         <v>0.3333333333333333</v>
@@ -1793,7 +1793,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Khmer</t>
+          <t>Mali</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1812,39 +1812,39 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Mapuche</t>
+          <t>Theodora</t>
         </is>
       </c>
       <c r="B73" t="n">
         <v>4</v>
       </c>
       <c r="C73" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D73" t="n">
-        <v>0.3076923076923077</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E73" t="n">
-        <v>1.692307692307692</v>
+        <v>1.666666666666667</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Yongle</t>
+          <t>Khmer</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D74" t="n">
-        <v>0.3</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E74" t="n">
-        <v>1.7</v>
+        <v>1.714285714285714</v>
       </c>
     </row>
     <row r="75">
@@ -1854,10 +1854,10 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C75" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D75" t="n">
         <v>0.2857142857142857</v>
@@ -1869,20 +1869,20 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Ludwig</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="B76" t="n">
         <v>2</v>
       </c>
       <c r="C76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D76" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.25</v>
       </c>
       <c r="E76" t="n">
-        <v>1.777777777777778</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="77">
@@ -1892,16 +1892,16 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="78">
@@ -1911,16 +1911,16 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>